<commit_message>
CAMBIOS EN FRONTEND Y BACKEND, SQL Y EXCEL
</commit_message>
<xml_diff>
--- a/datosseguros.xlsx
+++ b/datosseguros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angeldvvp\Desktop\prueba_chubb_AngelVergaraParedes_Viamatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8377CECC-1002-45E7-AC2F-067EF2F867BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D53152-5BD6-4E62-A287-74415DE195E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>CEDULA</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>0948746599</t>
+  </si>
+  <si>
+    <t>CODSEGURO</t>
+  </si>
+  <si>
+    <t>ADPR321000</t>
+  </si>
+  <si>
+    <t>SVPL543000</t>
+  </si>
+  <si>
+    <t>SGRC765000</t>
+  </si>
+  <si>
+    <t>GMYS432000,ADPR321000</t>
+  </si>
+  <si>
+    <t>ADPR321000,GMYS432000</t>
   </si>
 </sst>
 </file>
@@ -153,10 +171,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,9 +499,10 @@
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,8 +515,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -511,8 +532,11 @@
       <c r="D2">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,8 +549,11 @@
       <c r="D3">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -539,8 +566,11 @@
       <c r="D4">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -553,12 +583,15 @@
       <c r="D5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -568,7 +601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -581,8 +614,11 @@
       <c r="D7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -595,8 +631,11 @@
       <c r="D8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -610,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -622,6 +661,9 @@
       </c>
       <c r="D10">
         <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>